<commit_message>
created a get sched by dates function
</commit_message>
<xml_diff>
--- a/predict/2024/schedule/sched.xlsx
+++ b/predict/2024/schedule/sched.xlsx
@@ -3915,10 +3915,10 @@
         <v>464</v>
       </c>
       <c r="G74" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="H74" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="I74" t="s">
         <v>463</v>
@@ -4785,10 +4785,10 @@
         <v>464</v>
       </c>
       <c r="G104" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H104" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I104" t="s">
         <v>463</v>
@@ -8584,10 +8584,10 @@
         <v>464</v>
       </c>
       <c r="G235" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="H235" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="I235" t="s">
         <v>463</v>
@@ -9628,10 +9628,10 @@
         <v>464</v>
       </c>
       <c r="G271" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H271" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I271" t="s">
         <v>463</v>
@@ -10498,10 +10498,10 @@
         <v>464</v>
       </c>
       <c r="G301" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="H301" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="I301" t="s">
         <v>463</v>
@@ -12818,10 +12818,10 @@
         <v>464</v>
       </c>
       <c r="G381" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H381" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I381" t="s">
         <v>463</v>
@@ -13688,10 +13688,10 @@
         <v>464</v>
       </c>
       <c r="G411" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="H411" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="I411" t="s">
         <v>463</v>
@@ -16240,10 +16240,10 @@
         <v>464</v>
       </c>
       <c r="G499" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="H499" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="I499" t="s">
         <v>463</v>
@@ -16878,10 +16878,10 @@
         <v>464</v>
       </c>
       <c r="G521" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H521" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I521" t="s">
         <v>463</v>
@@ -18183,10 +18183,10 @@
         <v>464</v>
       </c>
       <c r="G566" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="H566" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="I566" t="s">
         <v>463</v>
@@ -19256,10 +19256,10 @@
         <v>464</v>
       </c>
       <c r="G603" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H603" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I603" t="s">
         <v>463</v>
@@ -24766,10 +24766,10 @@
         <v>464</v>
       </c>
       <c r="G793" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H793" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I793" t="s">
         <v>463</v>
@@ -26622,10 +26622,10 @@
         <v>464</v>
       </c>
       <c r="G857" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H857" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I857" t="s">
         <v>463</v>
@@ -28072,10 +28072,10 @@
         <v>464</v>
       </c>
       <c r="G907" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="H907" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="I907" t="s">
         <v>463</v>

</xml_diff>